<commit_message>
ME-models updated with ribosomal protein calling regardless of subunit information
</commit_message>
<xml_diff>
--- a/clean/lcrescens/building_data/automated-org-with-refs.xlsx
+++ b/clean/lcrescens/building_data/automated-org-with-refs.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25429" uniqueCount="6187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25431" uniqueCount="6187">
   <si>
     <t>Gene Locus ID</t>
   </si>
@@ -15025,10 +15025,10 @@
     <t>RNA_degradosome:1</t>
   </si>
   <si>
+    <t>ribosome:1</t>
+  </si>
+  <si>
     <t>translocation_pathway_srp</t>
-  </si>
-  <si>
-    <t>ribosome:1</t>
   </si>
   <si>
     <t>RNA_modifier_enzyme</t>
@@ -59003,6 +59003,9 @@
       <c r="I1243" t="s">
         <v>3683</v>
       </c>
+      <c r="L1243" t="s">
+        <v>5002</v>
+      </c>
       <c r="S1243" t="s">
         <v>6138</v>
       </c>
@@ -61130,6 +61133,9 @@
       <c r="I1363" t="s">
         <v>3801</v>
       </c>
+      <c r="L1363" t="s">
+        <v>5002</v>
+      </c>
       <c r="S1363" t="s">
         <v>6138</v>
       </c>
@@ -62011,7 +62017,7 @@
         <v>3848</v>
       </c>
       <c r="L1413" t="s">
-        <v>5002</v>
+        <v>5003</v>
       </c>
     </row>
     <row r="1414" spans="1:25">
@@ -62927,7 +62933,7 @@
         <v>3885</v>
       </c>
       <c r="L1460" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="1461" spans="1:19">
@@ -63073,7 +63079,7 @@
         <v>3889</v>
       </c>
       <c r="L1467" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="S1467" t="s">
         <v>6138</v>
@@ -64207,7 +64213,7 @@
         <v>3914</v>
       </c>
       <c r="L1518" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="S1518" t="s">
         <v>6138</v>
@@ -65384,7 +65390,7 @@
         <v>3936</v>
       </c>
       <c r="L1568" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="1569" spans="1:25">
@@ -66349,7 +66355,7 @@
         <v>3952</v>
       </c>
       <c r="L1611" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="1612" spans="1:25">
@@ -68834,7 +68840,7 @@
         <v>3979</v>
       </c>
       <c r="L1706" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="1707" spans="1:25">
@@ -69824,7 +69830,7 @@
         <v>4017</v>
       </c>
       <c r="L1757" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="1758" spans="1:25">
@@ -72868,7 +72874,7 @@
         <v>4996</v>
       </c>
       <c r="L1893" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="1894" spans="1:21">
@@ -73551,7 +73557,7 @@
         <v>4092</v>
       </c>
       <c r="L1927" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="1928" spans="1:19">
@@ -73591,7 +73597,7 @@
         <v>4094</v>
       </c>
       <c r="L1929" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="S1929" t="s">
         <v>6138</v>
@@ -73617,7 +73623,7 @@
         <v>4095</v>
       </c>
       <c r="L1930" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="1931" spans="1:19">
@@ -75676,7 +75682,7 @@
         <v>4150</v>
       </c>
       <c r="L2028" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="S2028" t="s">
         <v>6138</v>
@@ -75702,7 +75708,7 @@
         <v>4151</v>
       </c>
       <c r="L2029" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="S2029" t="s">
         <v>6138</v>
@@ -75777,7 +75783,7 @@
         <v>4154</v>
       </c>
       <c r="L2032" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="M2032" t="s">
         <v>5017</v>
@@ -75803,7 +75809,7 @@
         <v>4154</v>
       </c>
       <c r="L2033" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="M2033" t="s">
         <v>5018</v>
@@ -75829,7 +75835,7 @@
         <v>4155</v>
       </c>
       <c r="L2034" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="M2034" t="s">
         <v>5017</v>
@@ -75855,7 +75861,7 @@
         <v>4155</v>
       </c>
       <c r="L2035" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="M2035" t="s">
         <v>5018</v>
@@ -75881,7 +75887,7 @@
         <v>4156</v>
       </c>
       <c r="L2036" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="M2036" t="s">
         <v>5017</v>
@@ -75907,7 +75913,7 @@
         <v>4156</v>
       </c>
       <c r="L2037" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="M2037" t="s">
         <v>5018</v>
@@ -75933,7 +75939,7 @@
         <v>4157</v>
       </c>
       <c r="L2038" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="2039" spans="1:19">
@@ -75956,7 +75962,7 @@
         <v>4158</v>
       </c>
       <c r="L2039" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="S2039" t="s">
         <v>6138</v>
@@ -75982,7 +75988,7 @@
         <v>4159</v>
       </c>
       <c r="L2040" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="S2040" t="s">
         <v>6138</v>
@@ -76008,7 +76014,7 @@
         <v>4160</v>
       </c>
       <c r="L2041" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="2042" spans="1:19">
@@ -76031,7 +76037,7 @@
         <v>4161</v>
       </c>
       <c r="L2042" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="S2042" t="s">
         <v>6138</v>
@@ -76057,7 +76063,7 @@
         <v>4162</v>
       </c>
       <c r="L2043" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="2044" spans="1:19">
@@ -76080,7 +76086,7 @@
         <v>4163</v>
       </c>
       <c r="L2044" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="2045" spans="1:19">
@@ -76103,7 +76109,7 @@
         <v>4164</v>
       </c>
       <c r="L2045" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="S2045" t="s">
         <v>6138</v>
@@ -76129,7 +76135,7 @@
         <v>4165</v>
       </c>
       <c r="L2046" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="2047" spans="1:19">
@@ -76152,7 +76158,7 @@
         <v>4166</v>
       </c>
       <c r="L2047" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="S2047" t="s">
         <v>6138</v>
@@ -76178,7 +76184,7 @@
         <v>4167</v>
       </c>
       <c r="L2048" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="S2048" t="s">
         <v>6138</v>
@@ -76204,7 +76210,7 @@
         <v>4168</v>
       </c>
       <c r="L2049" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="S2049" t="s">
         <v>6138</v>
@@ -76230,7 +76236,7 @@
         <v>4169</v>
       </c>
       <c r="L2050" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="S2050" t="s">
         <v>6138</v>
@@ -76256,7 +76262,7 @@
         <v>4170</v>
       </c>
       <c r="L2051" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="S2051" t="s">
         <v>6138</v>
@@ -76282,7 +76288,7 @@
         <v>4171</v>
       </c>
       <c r="L2052" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="2053" spans="1:25">
@@ -76305,7 +76311,7 @@
         <v>4172</v>
       </c>
       <c r="L2053" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="S2053" t="s">
         <v>6138</v>
@@ -76328,7 +76334,7 @@
         <v>4173</v>
       </c>
       <c r="L2054" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="2055" spans="1:25">
@@ -76351,7 +76357,7 @@
         <v>4174</v>
       </c>
       <c r="L2055" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="2056" spans="1:25">
@@ -76446,7 +76452,7 @@
         <v>4176</v>
       </c>
       <c r="L2059" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="S2059" t="s">
         <v>6138</v>
@@ -76472,7 +76478,7 @@
         <v>4177</v>
       </c>
       <c r="L2060" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="S2060" t="s">
         <v>6138</v>
@@ -76524,7 +76530,7 @@
         <v>4179</v>
       </c>
       <c r="L2062" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="2063" spans="1:25">
@@ -76813,7 +76819,7 @@
         <v>4188</v>
       </c>
       <c r="L2076" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="2077" spans="1:21">
@@ -78084,7 +78090,7 @@
         <v>4246</v>
       </c>
       <c r="L2146" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="M2146" t="s">
         <v>5017</v>
@@ -78113,7 +78119,7 @@
         <v>4246</v>
       </c>
       <c r="L2147" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="M2147" t="s">
         <v>5018</v>
@@ -82474,7 +82480,7 @@
         <v>4361</v>
       </c>
       <c r="L2355" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="2356" spans="1:19">
@@ -85769,7 +85775,7 @@
         <v>4457</v>
       </c>
       <c r="L2516" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="S2516" t="s">
         <v>6138</v>
@@ -85838,7 +85844,7 @@
         <v>4459</v>
       </c>
       <c r="L2519" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="S2519" t="s">
         <v>6138</v>
@@ -85864,7 +85870,7 @@
         <v>4460</v>
       </c>
       <c r="L2520" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="S2520" t="s">
         <v>6138</v>
@@ -86343,7 +86349,7 @@
         <v>4471</v>
       </c>
       <c r="L2542" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="2543" spans="1:21">
@@ -87738,7 +87744,7 @@
         <v>4513</v>
       </c>
       <c r="L2614" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="M2614" t="s">
         <v>5017</v>
@@ -87764,7 +87770,7 @@
         <v>4513</v>
       </c>
       <c r="L2615" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="M2615" t="s">
         <v>5018</v>
@@ -87790,7 +87796,7 @@
         <v>4514</v>
       </c>
       <c r="L2616" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="S2616" t="s">
         <v>6138</v>
@@ -89327,7 +89333,7 @@
         <v>4996</v>
       </c>
       <c r="L2696" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="2697" spans="1:25">
@@ -90714,7 +90720,7 @@
         <v>4587</v>
       </c>
       <c r="L2758" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="2759" spans="1:25">
@@ -92283,7 +92289,7 @@
         <v>4619</v>
       </c>
       <c r="L2830" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="S2830" t="s">
         <v>6138</v>
@@ -92306,7 +92312,7 @@
         <v>4620</v>
       </c>
       <c r="L2831" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="2832" spans="1:21">
@@ -93883,7 +93889,7 @@
         <v>4655</v>
       </c>
       <c r="L2907" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="S2907" t="s">
         <v>6138</v>
@@ -95732,7 +95738,7 @@
         <v>4699</v>
       </c>
       <c r="L2993" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="S2993" t="s">
         <v>6138</v>
@@ -96250,7 +96256,7 @@
         <v>4711</v>
       </c>
       <c r="L3015" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="3016" spans="1:25">
@@ -96273,7 +96279,7 @@
         <v>4712</v>
       </c>
       <c r="L3016" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="S3016" t="s">
         <v>6138</v>
@@ -97637,7 +97643,7 @@
         <v>4757</v>
       </c>
       <c r="L3083" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="3084" spans="1:25">
@@ -97706,7 +97712,7 @@
         <v>4760</v>
       </c>
       <c r="L3086" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="S3086" t="s">
         <v>6138</v>
@@ -98985,7 +98991,7 @@
         <v>4796</v>
       </c>
       <c r="L3151" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="3152" spans="1:19">
@@ -99749,7 +99755,7 @@
         <v>4996</v>
       </c>
       <c r="L3188" t="s">
-        <v>5003</v>
+        <v>5002</v>
       </c>
     </row>
     <row r="3189" spans="1:21">

</xml_diff>